<commit_message>
update boms and gerbers
</commit_message>
<xml_diff>
--- a/Pikatea Macropad GB4/Gerbers/GB4 BOM.xlsx
+++ b/Pikatea Macropad GB4/Gerbers/GB4 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackr\Documents\KiCad\PikateaPCB\Pikatea Macropad GB4\Gerbers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7787581-106B-4CEE-A5B4-9C6C099D9A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160BA7A7-5B3C-4ADB-8F0C-A608C5974DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1032" windowWidth="23040" windowHeight="11328" xr2:uid="{5CBD5225-9053-409E-BB21-F66D4D8F4B94}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="11328" xr2:uid="{5CBD5225-9053-409E-BB21-F66D4D8F4B94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Id</t>
   </si>
@@ -116,15 +116,6 @@
   </si>
   <si>
     <t>ATMEGA32U4-EP</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>AVR_ICSP_3x2</t>
-  </si>
-  <si>
-    <t>AVR-ISP-6</t>
   </si>
   <si>
     <t>SW1</t>
@@ -524,7 +515,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,44 +692,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -746,22 +720,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -769,22 +743,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>